<commit_message>
plotting changes and slight reformatting
Changed around the colors of the t_set plots to go from Red (no) to Green (yes) with Yellow being neutral. Now matches up with the excel coloration. I also changed around a few things within the main forge code, essentially attempts to increase the common code base and decrease fault opportunities. The more I look at it the more I think it's in need of another reorganization, it's getting pretty unwieldy for a single file. I have marked a few places that things can be easily extracted out into util or a new graphing class. More work will need to be done. Perhaps even a forge superclass with state specific classes inheriting from it. A project for the summer. As is tradition now I've done a full recompile, thus the large commit
</commit_message>
<xml_diff>
--- a/data/IN/outputs/590034/t_set_test.xlsx
+++ b/data/IN/outputs/590034/t_set_test.xlsx
@@ -32,18 +32,624 @@
     <t>final</t>
   </si>
   <si>
+    <t>committee_vote</t>
+  </si>
+  <si>
+    <t>committee_consistency</t>
+  </si>
+  <si>
+    <t>p_yes_rev_cs</t>
+  </si>
+  <si>
+    <t>id5506</t>
+  </si>
+  <si>
+    <t>id5529</t>
+  </si>
+  <si>
+    <t>id12223</t>
+  </si>
+  <si>
+    <t>id5493</t>
+  </si>
+  <si>
+    <t>id14189</t>
+  </si>
+  <si>
+    <t>id5494</t>
+  </si>
+  <si>
+    <t>id5489</t>
+  </si>
+  <si>
+    <t>id5553</t>
+  </si>
+  <si>
+    <t>id5482</t>
+  </si>
+  <si>
+    <t>id5532</t>
+  </si>
+  <si>
+    <t>id14765</t>
+  </si>
+  <si>
+    <t>id5516</t>
+  </si>
+  <si>
+    <t>id14192</t>
+  </si>
+  <si>
+    <t>id5492</t>
+  </si>
+  <si>
+    <t>id14766</t>
+  </si>
+  <si>
+    <t>id5570</t>
+  </si>
+  <si>
+    <t>id14438</t>
+  </si>
+  <si>
+    <t>id5546</t>
+  </si>
+  <si>
+    <t>id5552</t>
+  </si>
+  <si>
+    <t>id5519</t>
+  </si>
+  <si>
+    <t>id11394</t>
+  </si>
+  <si>
+    <t>id10569</t>
+  </si>
+  <si>
+    <t>id5539</t>
+  </si>
+  <si>
+    <t>id14761</t>
+  </si>
+  <si>
+    <t>id5571</t>
+  </si>
+  <si>
+    <t>id5515</t>
+  </si>
+  <si>
+    <t>id5508</t>
+  </si>
+  <si>
+    <t>id5560</t>
+  </si>
+  <si>
+    <t>id5544</t>
+  </si>
+  <si>
+    <t>id10578</t>
+  </si>
+  <si>
+    <t>id10575</t>
+  </si>
+  <si>
+    <t>id5559</t>
+  </si>
+  <si>
+    <t>id5561</t>
+  </si>
+  <si>
+    <t>id5624</t>
+  </si>
+  <si>
+    <t>id5564</t>
+  </si>
+  <si>
+    <t>id5499</t>
+  </si>
+  <si>
+    <t>id14439</t>
+  </si>
+  <si>
+    <t>id10577</t>
+  </si>
+  <si>
+    <t>id5509</t>
+  </si>
+  <si>
+    <t>id5502</t>
+  </si>
+  <si>
+    <t>id5524</t>
+  </si>
+  <si>
+    <t>id14443</t>
+  </si>
+  <si>
+    <t>id5498</t>
+  </si>
+  <si>
+    <t>id10818</t>
+  </si>
+  <si>
+    <t>id5563</t>
+  </si>
+  <si>
+    <t>id10574</t>
+  </si>
+  <si>
+    <t>id14445</t>
+  </si>
+  <si>
+    <t>id5512</t>
+  </si>
+  <si>
+    <t>id5513</t>
+  </si>
+  <si>
+    <t>id5510</t>
+  </si>
+  <si>
+    <t>id14768</t>
+  </si>
+  <si>
+    <t>id14447</t>
+  </si>
+  <si>
+    <t>id5527</t>
+  </si>
+  <si>
+    <t>id5537</t>
+  </si>
+  <si>
+    <t>id14767</t>
+  </si>
+  <si>
+    <t>id14437</t>
+  </si>
+  <si>
+    <t>id5573</t>
+  </si>
+  <si>
+    <t>id5536</t>
+  </si>
+  <si>
+    <t>id10584</t>
+  </si>
+  <si>
+    <t>id14441</t>
+  </si>
+  <si>
+    <t>id5549</t>
+  </si>
+  <si>
+    <t>id10579</t>
+  </si>
+  <si>
+    <t>id5541</t>
+  </si>
+  <si>
+    <t>id14448</t>
+  </si>
+  <si>
+    <t>id5483</t>
+  </si>
+  <si>
+    <t>id5528</t>
+  </si>
+  <si>
+    <t>id10570</t>
+  </si>
+  <si>
+    <t>id10572</t>
+  </si>
+  <si>
+    <t>id14764</t>
+  </si>
+  <si>
+    <t>id10573</t>
+  </si>
+  <si>
+    <t>id5568</t>
+  </si>
+  <si>
+    <t>id5514</t>
+  </si>
+  <si>
+    <t>id10571</t>
+  </si>
+  <si>
+    <t>id11398</t>
+  </si>
+  <si>
+    <t>id10568</t>
+  </si>
+  <si>
+    <t>id11298</t>
+  </si>
+  <si>
+    <t>id5500</t>
+  </si>
+  <si>
+    <t>id5547</t>
+  </si>
+  <si>
+    <t>id5557</t>
+  </si>
+  <si>
+    <t>id5569</t>
+  </si>
+  <si>
+    <t>id14762</t>
+  </si>
+  <si>
+    <t>id14444</t>
+  </si>
+  <si>
+    <t>id10816</t>
+  </si>
+  <si>
+    <t>id10576</t>
+  </si>
+  <si>
+    <t>id5521</t>
+  </si>
+  <si>
+    <t>id5533</t>
+  </si>
+  <si>
+    <t>id14436</t>
+  </si>
+  <si>
+    <t>id5497</t>
+  </si>
+  <si>
+    <t>id11395</t>
+  </si>
+  <si>
+    <t>id11396</t>
+  </si>
+  <si>
+    <t>id5567</t>
+  </si>
+  <si>
+    <t>id14440</t>
+  </si>
+  <si>
+    <t>id5565</t>
+  </si>
+  <si>
+    <t>id5543</t>
+  </si>
+  <si>
+    <t>id5556</t>
+  </si>
+  <si>
+    <t>id5566</t>
+  </si>
+  <si>
+    <t>id14442</t>
+  </si>
+  <si>
+    <t>id14446</t>
+  </si>
+  <si>
+    <t>id5518</t>
+  </si>
+  <si>
+    <t>id14191</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Linda Lawson</t>
+  </si>
+  <si>
+    <t>Earl Harris</t>
+  </si>
+  <si>
+    <t>Charlie Brown</t>
+  </si>
+  <si>
+    <t>Edmond Soliday</t>
+  </si>
+  <si>
+    <t>Dale DeVon</t>
+  </si>
+  <si>
+    <t>Patrick Bauer</t>
+  </si>
+  <si>
+    <t>David Niezgodski</t>
+  </si>
+  <si>
+    <t>Ryan Dvorak</t>
+  </si>
+  <si>
+    <t>Scott Pelath</t>
+  </si>
+  <si>
+    <t>Charles Moseley</t>
+  </si>
+  <si>
+    <t>Rick Niemeyer</t>
+  </si>
+  <si>
+    <t>Mara Reardon</t>
+  </si>
+  <si>
+    <t>Sharon Negele</t>
+  </si>
+  <si>
+    <t>Vernon Smith</t>
+  </si>
+  <si>
+    <t>Harold Slager</t>
+  </si>
+  <si>
+    <t>Doug Gutwein</t>
+  </si>
+  <si>
+    <t>Timothy Harman</t>
+  </si>
+  <si>
+    <t>David Wolkins</t>
+  </si>
+  <si>
+    <t>Rochelle VanDenburgh</t>
+  </si>
+  <si>
+    <t>Thomas Dermody</t>
+  </si>
+  <si>
+    <t>Timothy Wesco</t>
+  </si>
+  <si>
+    <t>Rebecca Kubacki</t>
+  </si>
+  <si>
+    <t>William Friend</t>
+  </si>
+  <si>
+    <t>Steven Braun</t>
+  </si>
+  <si>
+    <t>Donald Lehe</t>
+  </si>
+  <si>
+    <t>Randy Truitt</t>
+  </si>
+  <si>
+    <t>Sheila Klinker</t>
+  </si>
+  <si>
+    <t>Jeffrey Thompson</t>
+  </si>
+  <si>
+    <t>Kathy Richardson</t>
+  </si>
+  <si>
+    <t>Michael Karickhoff</t>
+  </si>
+  <si>
+    <t>Kevin Mahan</t>
+  </si>
+  <si>
+    <t>Eric Turner</t>
+  </si>
+  <si>
+    <t>Bill Davis</t>
+  </si>
+  <si>
+    <t>Sue Errington</t>
+  </si>
+  <si>
+    <t>Jack Lutz</t>
+  </si>
+  <si>
+    <t>Terri Jo Austin</t>
+  </si>
+  <si>
+    <t>Todd Huston</t>
+  </si>
+  <si>
+    <t>Heath VanNatter</t>
+  </si>
+  <si>
+    <t>Gerald Torr</t>
+  </si>
+  <si>
+    <t>Gregory Steuerwald</t>
+  </si>
+  <si>
+    <t>Timothy Brown</t>
+  </si>
+  <si>
+    <t>Alan Morrison</t>
+  </si>
+  <si>
+    <t>Clyde Kersey</t>
+  </si>
+  <si>
+    <t>James Baird</t>
+  </si>
+  <si>
+    <t>Kreg Battles</t>
+  </si>
+  <si>
+    <t>Robert Heaton</t>
+  </si>
+  <si>
+    <t>John Price</t>
+  </si>
+  <si>
+    <t>Timothy Neese</t>
+  </si>
+  <si>
+    <t>Wes Culver</t>
+  </si>
+  <si>
+    <t>Daniel Leonard</t>
+  </si>
+  <si>
+    <t>Dennis Zent</t>
+  </si>
+  <si>
+    <t>Ben Smaltz</t>
+  </si>
+  <si>
+    <t>Robert Cherry</t>
+  </si>
+  <si>
+    <t>Thomas Saunders</t>
+  </si>
+  <si>
+    <t>Cindy Ziemke</t>
+  </si>
+  <si>
+    <t>Richard Hamm</t>
+  </si>
+  <si>
+    <t>Sean Eberhart</t>
+  </si>
+  <si>
+    <t>Charles Burton</t>
+  </si>
+  <si>
+    <t>Milo Smith</t>
+  </si>
+  <si>
+    <t>Peggy Mayfield</t>
+  </si>
+  <si>
+    <t>Matt Pierce</t>
+  </si>
+  <si>
+    <t>Matthew Ubelhor</t>
+  </si>
+  <si>
+    <t>Mark Messmer</t>
+  </si>
+  <si>
+    <t>Thomas Washburne</t>
+  </si>
+  <si>
+    <t>Eric Koch</t>
+  </si>
+  <si>
+    <t>Terry Goodin</t>
+  </si>
+  <si>
+    <t>Randall Frye</t>
+  </si>
+  <si>
+    <t>Judson McMillin</t>
+  </si>
+  <si>
+    <t>Jim Lucas</t>
+  </si>
+  <si>
+    <t>Rhonda Rhoads</t>
+  </si>
+  <si>
+    <t>Steven Stemler</t>
+  </si>
+  <si>
+    <t>Edward Clere</t>
+  </si>
+  <si>
+    <t>Steven Davisson</t>
+  </si>
+  <si>
+    <t>Lloyd Arnold</t>
+  </si>
+  <si>
+    <t>Ronald Bacon</t>
+  </si>
+  <si>
+    <t>Wendy McNamara</t>
+  </si>
+  <si>
+    <t>Gail Riecken</t>
+  </si>
+  <si>
+    <t>Suzanne Crouch</t>
+  </si>
+  <si>
+    <t>Matthew Lehman</t>
+  </si>
+  <si>
+    <t>Philip GiaQuinta</t>
+  </si>
+  <si>
+    <t>Martin Carbaugh</t>
+  </si>
+  <si>
+    <t>David Ober</t>
+  </si>
+  <si>
+    <t>Kathleen Heuer</t>
+  </si>
+  <si>
+    <t>Robert Morris</t>
+  </si>
+  <si>
+    <t>Phyllis Pond</t>
+  </si>
+  <si>
+    <t>Edward DeLaney</t>
+  </si>
+  <si>
+    <t>Christina Hale</t>
+  </si>
+  <si>
+    <t>Brian Bosma</t>
+  </si>
+  <si>
+    <t>Cindy Kirchhofer</t>
+  </si>
+  <si>
+    <t>Mike Speedy</t>
+  </si>
+  <si>
+    <t>Robert Behning</t>
+  </si>
+  <si>
+    <t>Karlee Macer</t>
+  </si>
+  <si>
+    <t>David Frizzell</t>
+  </si>
+  <si>
+    <t>Cherrish Pryor</t>
+  </si>
+  <si>
+    <t>John Bartlett</t>
+  </si>
+  <si>
+    <t>Gregory Porter</t>
+  </si>
+  <si>
+    <t>Justin Moed</t>
+  </si>
+  <si>
+    <t>Robin Shackleford</t>
+  </si>
+  <si>
+    <t>Vanessa Summers</t>
+  </si>
+  <si>
+    <t>Dan Forestal</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
     <t>t1</t>
   </si>
   <si>
-    <t>committee_vote</t>
-  </si>
-  <si>
-    <t>committee_consistency</t>
-  </si>
-  <si>
-    <t>p_yes_rev_cs</t>
-  </si>
-  <si>
     <t>t2</t>
   </si>
   <si>
@@ -56,304 +662,7 @@
     <t>t5</t>
   </si>
   <si>
-    <t>id5506</t>
-  </si>
-  <si>
-    <t>id5529</t>
-  </si>
-  <si>
-    <t>id12223</t>
-  </si>
-  <si>
-    <t>id5493</t>
-  </si>
-  <si>
-    <t>id14189</t>
-  </si>
-  <si>
-    <t>id5494</t>
-  </si>
-  <si>
-    <t>id5489</t>
-  </si>
-  <si>
-    <t>id5553</t>
-  </si>
-  <si>
-    <t>id5482</t>
-  </si>
-  <si>
-    <t>id5532</t>
-  </si>
-  <si>
-    <t>id14765</t>
-  </si>
-  <si>
-    <t>id5516</t>
-  </si>
-  <si>
-    <t>id14192</t>
-  </si>
-  <si>
-    <t>id5492</t>
-  </si>
-  <si>
-    <t>id14766</t>
-  </si>
-  <si>
-    <t>id5570</t>
-  </si>
-  <si>
-    <t>id14438</t>
-  </si>
-  <si>
-    <t>id5546</t>
-  </si>
-  <si>
-    <t>id5552</t>
-  </si>
-  <si>
-    <t>id5519</t>
-  </si>
-  <si>
-    <t>id11394</t>
-  </si>
-  <si>
-    <t>id10569</t>
-  </si>
-  <si>
-    <t>id5539</t>
-  </si>
-  <si>
-    <t>id14761</t>
-  </si>
-  <si>
-    <t>id5571</t>
-  </si>
-  <si>
-    <t>id5515</t>
-  </si>
-  <si>
-    <t>id5508</t>
-  </si>
-  <si>
-    <t>id5560</t>
-  </si>
-  <si>
-    <t>id5544</t>
-  </si>
-  <si>
-    <t>id10578</t>
-  </si>
-  <si>
-    <t>id10575</t>
-  </si>
-  <si>
-    <t>id5559</t>
-  </si>
-  <si>
-    <t>id5561</t>
-  </si>
-  <si>
-    <t>id5624</t>
-  </si>
-  <si>
-    <t>id5564</t>
-  </si>
-  <si>
-    <t>id5499</t>
-  </si>
-  <si>
-    <t>id14439</t>
-  </si>
-  <si>
-    <t>id10577</t>
-  </si>
-  <si>
-    <t>id5509</t>
-  </si>
-  <si>
-    <t>id5502</t>
-  </si>
-  <si>
-    <t>id5524</t>
-  </si>
-  <si>
-    <t>id14443</t>
-  </si>
-  <si>
-    <t>id5498</t>
-  </si>
-  <si>
-    <t>id10818</t>
-  </si>
-  <si>
-    <t>id5563</t>
-  </si>
-  <si>
-    <t>id10574</t>
-  </si>
-  <si>
-    <t>id14445</t>
-  </si>
-  <si>
-    <t>id5512</t>
-  </si>
-  <si>
-    <t>id5513</t>
-  </si>
-  <si>
-    <t>id5510</t>
-  </si>
-  <si>
-    <t>id14768</t>
-  </si>
-  <si>
-    <t>id14447</t>
-  </si>
-  <si>
-    <t>id5527</t>
-  </si>
-  <si>
-    <t>id5537</t>
-  </si>
-  <si>
-    <t>id14767</t>
-  </si>
-  <si>
-    <t>id14437</t>
-  </si>
-  <si>
-    <t>id5573</t>
-  </si>
-  <si>
-    <t>id5536</t>
-  </si>
-  <si>
-    <t>id10584</t>
-  </si>
-  <si>
-    <t>id14441</t>
-  </si>
-  <si>
-    <t>id5549</t>
-  </si>
-  <si>
-    <t>id10579</t>
-  </si>
-  <si>
-    <t>id5541</t>
-  </si>
-  <si>
-    <t>id14448</t>
-  </si>
-  <si>
-    <t>id5483</t>
-  </si>
-  <si>
-    <t>id5528</t>
-  </si>
-  <si>
-    <t>id10570</t>
-  </si>
-  <si>
-    <t>id10572</t>
-  </si>
-  <si>
-    <t>id14764</t>
-  </si>
-  <si>
-    <t>id10573</t>
-  </si>
-  <si>
-    <t>id5568</t>
-  </si>
-  <si>
-    <t>id5514</t>
-  </si>
-  <si>
-    <t>id10571</t>
-  </si>
-  <si>
-    <t>id11398</t>
-  </si>
-  <si>
-    <t>id10568</t>
-  </si>
-  <si>
-    <t>id11298</t>
-  </si>
-  <si>
-    <t>id5500</t>
-  </si>
-  <si>
-    <t>id5547</t>
-  </si>
-  <si>
-    <t>id5557</t>
-  </si>
-  <si>
-    <t>id5569</t>
-  </si>
-  <si>
-    <t>id14762</t>
-  </si>
-  <si>
-    <t>id14444</t>
-  </si>
-  <si>
-    <t>id10816</t>
-  </si>
-  <si>
-    <t>id10576</t>
-  </si>
-  <si>
-    <t>id5521</t>
-  </si>
-  <si>
-    <t>id5533</t>
-  </si>
-  <si>
-    <t>id14436</t>
-  </si>
-  <si>
-    <t>id5497</t>
-  </si>
-  <si>
-    <t>id11395</t>
-  </si>
-  <si>
-    <t>id11396</t>
-  </si>
-  <si>
-    <t>id5567</t>
-  </si>
-  <si>
-    <t>id14440</t>
-  </si>
-  <si>
-    <t>id5565</t>
-  </si>
-  <si>
-    <t>id5543</t>
-  </si>
-  <si>
-    <t>id5556</t>
-  </si>
-  <si>
-    <t>id5566</t>
-  </si>
-  <si>
-    <t>id14442</t>
-  </si>
-  <si>
-    <t>id14446</t>
-  </si>
-  <si>
-    <t>id5518</t>
-  </si>
-  <si>
-    <t>id14191</t>
+    <t>t6</t>
   </si>
   <si>
     <t>t7</t>
@@ -383,6 +692,9 @@
     <t>t15</t>
   </si>
   <si>
+    <t>t16</t>
+  </si>
+  <si>
     <t>t17</t>
   </si>
   <si>
@@ -390,318 +702,6 @@
   </si>
   <si>
     <t>t18_check</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Linda Lawson</t>
-  </si>
-  <si>
-    <t>Earl Harris</t>
-  </si>
-  <si>
-    <t>Charlie Brown</t>
-  </si>
-  <si>
-    <t>Edmond Soliday</t>
-  </si>
-  <si>
-    <t>Dale DeVon</t>
-  </si>
-  <si>
-    <t>Patrick Bauer</t>
-  </si>
-  <si>
-    <t>David Niezgodski</t>
-  </si>
-  <si>
-    <t>Ryan Dvorak</t>
-  </si>
-  <si>
-    <t>Scott Pelath</t>
-  </si>
-  <si>
-    <t>Charles Moseley</t>
-  </si>
-  <si>
-    <t>Rick Niemeyer</t>
-  </si>
-  <si>
-    <t>Mara Reardon</t>
-  </si>
-  <si>
-    <t>Sharon Negele</t>
-  </si>
-  <si>
-    <t>Vernon Smith</t>
-  </si>
-  <si>
-    <t>Harold Slager</t>
-  </si>
-  <si>
-    <t>Doug Gutwein</t>
-  </si>
-  <si>
-    <t>Timothy Harman</t>
-  </si>
-  <si>
-    <t>David Wolkins</t>
-  </si>
-  <si>
-    <t>Rochelle VanDenburgh</t>
-  </si>
-  <si>
-    <t>Thomas Dermody</t>
-  </si>
-  <si>
-    <t>Timothy Wesco</t>
-  </si>
-  <si>
-    <t>Rebecca Kubacki</t>
-  </si>
-  <si>
-    <t>William Friend</t>
-  </si>
-  <si>
-    <t>Steven Braun</t>
-  </si>
-  <si>
-    <t>Donald Lehe</t>
-  </si>
-  <si>
-    <t>Randy Truitt</t>
-  </si>
-  <si>
-    <t>Sheila Klinker</t>
-  </si>
-  <si>
-    <t>Jeffrey Thompson</t>
-  </si>
-  <si>
-    <t>Kathy Richardson</t>
-  </si>
-  <si>
-    <t>Michael Karickhoff</t>
-  </si>
-  <si>
-    <t>Kevin Mahan</t>
-  </si>
-  <si>
-    <t>Eric Turner</t>
-  </si>
-  <si>
-    <t>Bill Davis</t>
-  </si>
-  <si>
-    <t>Sue Errington</t>
-  </si>
-  <si>
-    <t>Jack Lutz</t>
-  </si>
-  <si>
-    <t>Terri Jo Austin</t>
-  </si>
-  <si>
-    <t>Todd Huston</t>
-  </si>
-  <si>
-    <t>Heath VanNatter</t>
-  </si>
-  <si>
-    <t>Gerald Torr</t>
-  </si>
-  <si>
-    <t>Gregory Steuerwald</t>
-  </si>
-  <si>
-    <t>Timothy Brown</t>
-  </si>
-  <si>
-    <t>Alan Morrison</t>
-  </si>
-  <si>
-    <t>Clyde Kersey</t>
-  </si>
-  <si>
-    <t>James Baird</t>
-  </si>
-  <si>
-    <t>Kreg Battles</t>
-  </si>
-  <si>
-    <t>Robert Heaton</t>
-  </si>
-  <si>
-    <t>John Price</t>
-  </si>
-  <si>
-    <t>Timothy Neese</t>
-  </si>
-  <si>
-    <t>Wes Culver</t>
-  </si>
-  <si>
-    <t>Daniel Leonard</t>
-  </si>
-  <si>
-    <t>Dennis Zent</t>
-  </si>
-  <si>
-    <t>Ben Smaltz</t>
-  </si>
-  <si>
-    <t>Robert Cherry</t>
-  </si>
-  <si>
-    <t>Thomas Saunders</t>
-  </si>
-  <si>
-    <t>Cindy Ziemke</t>
-  </si>
-  <si>
-    <t>Richard Hamm</t>
-  </si>
-  <si>
-    <t>Sean Eberhart</t>
-  </si>
-  <si>
-    <t>Charles Burton</t>
-  </si>
-  <si>
-    <t>Milo Smith</t>
-  </si>
-  <si>
-    <t>Peggy Mayfield</t>
-  </si>
-  <si>
-    <t>Matt Pierce</t>
-  </si>
-  <si>
-    <t>Matthew Ubelhor</t>
-  </si>
-  <si>
-    <t>Mark Messmer</t>
-  </si>
-  <si>
-    <t>Thomas Washburne</t>
-  </si>
-  <si>
-    <t>Eric Koch</t>
-  </si>
-  <si>
-    <t>Terry Goodin</t>
-  </si>
-  <si>
-    <t>Randall Frye</t>
-  </si>
-  <si>
-    <t>Judson McMillin</t>
-  </si>
-  <si>
-    <t>Jim Lucas</t>
-  </si>
-  <si>
-    <t>Rhonda Rhoads</t>
-  </si>
-  <si>
-    <t>Steven Stemler</t>
-  </si>
-  <si>
-    <t>Edward Clere</t>
-  </si>
-  <si>
-    <t>Steven Davisson</t>
-  </si>
-  <si>
-    <t>Lloyd Arnold</t>
-  </si>
-  <si>
-    <t>Ronald Bacon</t>
-  </si>
-  <si>
-    <t>Wendy McNamara</t>
-  </si>
-  <si>
-    <t>Gail Riecken</t>
-  </si>
-  <si>
-    <t>Suzanne Crouch</t>
-  </si>
-  <si>
-    <t>Matthew Lehman</t>
-  </si>
-  <si>
-    <t>Philip GiaQuinta</t>
-  </si>
-  <si>
-    <t>Martin Carbaugh</t>
-  </si>
-  <si>
-    <t>David Ober</t>
-  </si>
-  <si>
-    <t>Kathleen Heuer</t>
-  </si>
-  <si>
-    <t>Robert Morris</t>
-  </si>
-  <si>
-    <t>Phyllis Pond</t>
-  </si>
-  <si>
-    <t>Edward DeLaney</t>
-  </si>
-  <si>
-    <t>Christina Hale</t>
-  </si>
-  <si>
-    <t>Brian Bosma</t>
-  </si>
-  <si>
-    <t>Cindy Kirchhofer</t>
-  </si>
-  <si>
-    <t>Mike Speedy</t>
-  </si>
-  <si>
-    <t>Robert Behning</t>
-  </si>
-  <si>
-    <t>Karlee Macer</t>
-  </si>
-  <si>
-    <t>David Frizzell</t>
-  </si>
-  <si>
-    <t>Cherrish Pryor</t>
-  </si>
-  <si>
-    <t>John Bartlett</t>
-  </si>
-  <si>
-    <t>Gregory Porter</t>
-  </si>
-  <si>
-    <t>Justin Moed</t>
-  </si>
-  <si>
-    <t>Robin Shackleford</t>
-  </si>
-  <si>
-    <t>Vanessa Summers</t>
-  </si>
-  <si>
-    <t>Dan Forestal</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>t16</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X106" sqref="X106"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:Y102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,84 +1073,84 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="L1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O1" t="s">
+        <v>215</v>
+      </c>
+      <c r="P1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>217</v>
+      </c>
+      <c r="R1" t="s">
+        <v>218</v>
+      </c>
+      <c r="S1" t="s">
+        <v>219</v>
+      </c>
+      <c r="T1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U1" t="s">
+        <v>221</v>
+      </c>
+      <c r="V1" t="s">
+        <v>222</v>
+      </c>
+      <c r="W1" t="s">
+        <v>223</v>
+      </c>
+      <c r="X1" t="s">
         <v>224</v>
       </c>
-      <c r="M1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>114</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S1" t="s">
-        <v>116</v>
-      </c>
-      <c r="T1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" t="s">
-        <v>118</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>225</v>
-      </c>
-      <c r="W1" t="s">
-        <v>119</v>
-      </c>
-      <c r="X1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="H2">
         <v>0.9265318675509735</v>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="H3">
         <v>0.97106352690912112</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="H4">
         <v>0.12432418316594242</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="H5">
         <v>0.99999993579848012</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="H6">
         <v>0.99999990011524931</v>
@@ -1469,13 +1469,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="H7">
         <v>0.5968856395075427</v>
@@ -1534,13 +1534,13 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="H9">
         <v>0.81600585198408482</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="H10">
         <v>0.79446508478510991</v>
@@ -1741,13 +1741,13 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D11">
         <v>0.5</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="H12">
         <v>0.99998484918290231</v>
@@ -1883,13 +1883,13 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="H13">
         <v>0.72361950462518354</v>
@@ -1948,13 +1948,13 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="H14">
         <v>0.99999977848486898</v>
@@ -2013,13 +2013,13 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="H15">
         <v>0.23153424794410402</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="H16">
         <v>0.99999978398243894</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D17">
         <v>0.5</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="H18">
         <v>0.99998523226320846</v>
@@ -2285,13 +2285,13 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="H19">
         <v>0.99999983769565559</v>
@@ -2350,13 +2350,13 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="H20">
         <v>0.88631724880640117</v>
@@ -2415,13 +2415,13 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="H21">
         <v>0.99999977468596113</v>
@@ -2480,13 +2480,13 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D22">
         <v>0.99989798000408092</v>
@@ -2557,13 +2557,13 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D23">
         <v>0.99999793878394438</v>
@@ -2634,13 +2634,13 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="H24">
         <v>0.9999999936189724</v>
@@ -2699,13 +2699,13 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="H25">
         <v>0.99999997656461792</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="H26">
         <v>0.99999996185680229</v>
@@ -2829,13 +2829,13 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="H27">
         <v>0.99999974259839253</v>
@@ -2894,13 +2894,13 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="H28">
         <v>0.99983685625336405</v>
@@ -2959,13 +2959,13 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="H29">
         <v>0.99999002935699355</v>
@@ -3024,13 +3024,13 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="H30">
         <v>0.99999989945390788</v>
@@ -3089,13 +3089,13 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="H31">
         <v>0.99999988925159722</v>
@@ -3154,13 +3154,13 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="H32">
         <v>0.99999996320180762</v>
@@ -3219,13 +3219,13 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="H33">
         <v>0.99999989072094408</v>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="H34">
         <v>0.99999700486604315</v>
@@ -3346,13 +3346,13 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="H35">
         <v>0.98173494369833492</v>
@@ -3411,13 +3411,13 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="H36">
         <v>0.99999998022239944</v>
@@ -3476,13 +3476,13 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="H37">
         <v>0.98466013377815287</v>
@@ -3541,13 +3541,13 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="H38">
         <v>0.99999878615234439</v>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="H39">
         <v>0.99999961987764174</v>
@@ -3671,13 +3671,13 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D40">
         <v>0.99999793878394438</v>
@@ -3748,10 +3748,10 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="H41">
         <v>0.99999949630278817</v>
@@ -3810,10 +3810,10 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="H42">
         <v>0.99999895328391819</v>
@@ -3872,13 +3872,13 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="H43">
         <v>0.99999697391614195</v>
@@ -3937,13 +3937,13 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="H44">
         <v>0.85740647154505312</v>
@@ -4002,13 +4002,13 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="H45">
         <v>0.99999985503973898</v>
@@ -4067,13 +4067,13 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="H46">
         <v>0.99686166838859436</v>
@@ -4132,13 +4132,13 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="H47">
         <v>0.99999998275587876</v>
@@ -4197,13 +4197,13 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D48">
         <v>0.5</v>
@@ -4274,13 +4274,13 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="H49">
         <v>0.99999175393499917</v>
@@ -4339,13 +4339,13 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="H50">
         <v>0.99999974400174574</v>
@@ -4404,13 +4404,13 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="G51">
         <v>0.99</v>
@@ -4472,13 +4472,13 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="H52">
         <v>0.99999935259051909</v>
@@ -4537,13 +4537,13 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="H53">
         <v>0.99999976099671284</v>
@@ -4602,13 +4602,13 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="H54">
         <v>0.99999995408251408</v>
@@ -4667,13 +4667,13 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="H55">
         <v>0.99986877450516065</v>
@@ -4732,13 +4732,13 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="H56">
         <v>0.99999999561122654</v>
@@ -4797,13 +4797,13 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="G57">
         <v>0.99</v>
@@ -4865,13 +4865,13 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="H58">
         <v>0.9999906419468737</v>
@@ -4930,13 +4930,13 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="H59">
         <v>0.99999996026838311</v>
@@ -4995,13 +4995,13 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="H60">
         <v>0.99999997852930655</v>
@@ -5060,13 +5060,13 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="H61">
         <v>0.99999891948718156</v>
@@ -5125,13 +5125,13 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="H62">
         <v>0.54857079486476823</v>
@@ -5190,13 +5190,13 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="H63">
         <v>0.99999946216092006</v>
@@ -5255,13 +5255,13 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="H64">
         <v>0.9999998895115062</v>
@@ -5320,13 +5320,13 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="H65">
         <v>0.99996941224082325</v>
@@ -5385,13 +5385,13 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="H66">
         <v>0.99999888734513276</v>
@@ -5450,10 +5450,10 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="H67">
         <v>0.98851039883683234</v>
@@ -5512,13 +5512,13 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="H68">
         <v>0.99999872375233845</v>
@@ -5577,13 +5577,13 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H69">
         <v>0.99999942463596336</v>
@@ -5642,13 +5642,13 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="H70">
         <v>0.99999974141230008</v>
@@ -5707,13 +5707,13 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="H71">
         <v>0.999999956029474</v>
@@ -5772,10 +5772,10 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="H72">
         <v>0.99996147264010604</v>
@@ -5834,13 +5834,13 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="H73">
         <v>0.99999999042361787</v>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="H74">
         <v>0.99999757445402726</v>
@@ -5961,13 +5961,13 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B75">
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="H75">
         <v>0.99998401536431691</v>
@@ -6026,13 +6026,13 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="H76">
         <v>0.99999765137122687</v>
@@ -6091,13 +6091,13 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="H77">
         <v>0.99999969766594943</v>
@@ -6156,13 +6156,13 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="H78">
         <v>0.98276439209756128</v>
@@ -6221,10 +6221,10 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C79" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="H79">
         <v>0.99999976292465698</v>
@@ -6283,13 +6283,13 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="H80">
         <v>0.99999998973265347</v>
@@ -6348,13 +6348,13 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="G81">
         <v>0.66666666666666663</v>
@@ -6416,13 +6416,13 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="D82">
         <v>0.99999896939091004</v>
@@ -6493,13 +6493,13 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D83">
         <v>0.99999998958979652</v>
@@ -6570,13 +6570,13 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="H84">
         <v>0.99999998730810602</v>
@@ -6635,13 +6635,13 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="G85">
         <v>0.99</v>
@@ -6703,10 +6703,10 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C86" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="H86">
         <v>0.99999997333232438</v>
@@ -6765,13 +6765,13 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="H87">
         <v>0.67530747248482215</v>
@@ -6830,13 +6830,13 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="H88">
         <v>0.99771642341465905</v>
@@ -6895,10 +6895,10 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="H89">
         <v>0.99999999994837463</v>
@@ -6957,13 +6957,13 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B90">
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="H90">
         <v>0.99999997898257942</v>
@@ -7022,13 +7022,13 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="H91">
         <v>0.999999982395811</v>
@@ -7087,13 +7087,13 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="H92">
         <v>0.99999990210015399</v>
@@ -7152,10 +7152,10 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C93" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="H93">
         <v>0.97465996048630055</v>
@@ -7214,13 +7214,13 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="H94">
         <v>0.99999985363769672</v>
@@ -7279,13 +7279,13 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="H95">
         <v>0.17535058075722912</v>
@@ -7344,13 +7344,13 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="D96">
         <v>0.5</v>
@@ -7421,13 +7421,13 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="H97">
         <v>0.34824942765478789</v>
@@ -7486,13 +7486,13 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="H98">
         <v>0.99831766788679244</v>
@@ -7551,13 +7551,13 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="H99">
         <v>0.68774256251039589</v>
@@ -7616,13 +7616,13 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="H100">
         <v>0.68044923909885324</v>
@@ -7681,13 +7681,13 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="D101">
         <v>0.99999793878394438</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="H102">
         <v>77.777777777777786</v>

</xml_diff>